<commit_message>
Estadisticas trabajo y control de cambios
</commit_message>
<xml_diff>
--- a/01 - Planificacion del Trabajo/estadisticoHorasEmpleadas.xlsx
+++ b/01 - Planificacion del Trabajo/estadisticoHorasEmpleadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrés Martín Yeves\Desktop\TP1\SE\TP1SE\01 - Planificacion del Trabajo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/1er Cuatrimestre/TALLER PROYECTOS/SE/TP1SE/01 - Planificacion del Trabajo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66C8CB2-5E47-498A-A2A5-DE326516DC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901A9235-954B-0241-B9A7-1E7CD4244CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -391,6 +391,15 @@
                 <c:pt idx="120">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="122">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -523,6 +532,12 @@
                 <c:pt idx="120">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="123">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>3.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -655,6 +670,12 @@
                 <c:pt idx="120">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>3.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -816,6 +837,12 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1886,7 +1913,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1896,19 +1923,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57A6FB7-D46D-488C-A966-0ADB5C61A67C}">
   <dimension ref="E1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L126" sqref="L126"/>
+      <selection pane="bottomLeft" activeCell="G145" sqref="G145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="6" width="11.5546875" customWidth="1"/>
+    <col min="4" max="6" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
         <v>1</v>
       </c>
@@ -1925,25 +1952,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F4" t="s">
         <v>1</v>
       </c>
@@ -1960,7 +1987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E5" s="1"/>
       <c r="F5" s="3">
         <v>44826</v>
@@ -1976,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E6" s="1"/>
       <c r="F6" s="3">
         <v>44827</v>
@@ -1991,42 +2018,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F7" s="3">
         <v>44828</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F8" s="3">
         <v>44829</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F9" s="3">
         <v>44830</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F10" s="3">
         <v>44831</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F11" s="3">
         <v>44832</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F12" s="3">
         <v>44833</v>
       </c>
@@ -2043,7 +2070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F13" s="3">
         <v>44834</v>
       </c>
@@ -2055,28 +2082,28 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F14" s="3">
         <v>44835</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F15" s="3">
         <v>44836</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:10" x14ac:dyDescent="0.2">
       <c r="F16" s="3">
         <v>44837</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F17" s="3">
         <v>44838</v>
       </c>
@@ -2093,14 +2120,14 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F18" s="3">
         <v>44839</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F19" s="3">
         <v>44840</v>
       </c>
@@ -2117,35 +2144,35 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F20" s="3">
         <v>44841</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F21" s="3">
         <v>44842</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F22" s="3">
         <v>44843</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F23" s="3">
         <v>44844</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F24" s="3">
         <v>44845</v>
       </c>
@@ -2160,14 +2187,14 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F25" s="3">
         <v>44846</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F26" s="3">
         <v>44847</v>
       </c>
@@ -2184,7 +2211,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F27" s="3">
         <v>44848</v>
       </c>
@@ -2195,28 +2222,28 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F28" s="3">
         <v>44849</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F29" s="3">
         <v>44850</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F30" s="3">
         <v>44851</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F31" s="3">
         <v>44852</v>
       </c>
@@ -2233,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F32" s="3">
         <v>44853</v>
       </c>
@@ -2243,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F33" s="3">
         <v>44854</v>
       </c>
@@ -2260,7 +2287,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F34" s="3">
         <v>44855</v>
       </c>
@@ -2269,42 +2296,42 @@
       </c>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F35" s="3">
         <v>44856</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F36" s="3">
         <v>44857</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F37" s="3">
         <v>44858</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F38" s="3">
         <v>44859</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F39" s="3">
         <v>44860</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F40" s="3">
         <v>44861</v>
       </c>
@@ -2321,7 +2348,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="41" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F41" s="3">
         <v>44862</v>
       </c>
@@ -2331,7 +2358,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F42" s="3">
         <v>44863</v>
       </c>
@@ -2341,35 +2368,35 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="43" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F43" s="3">
         <v>44864</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F44" s="3">
         <v>44865</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F45" s="3">
         <v>44866</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F46" s="3">
         <v>44867</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F47" s="3">
         <v>44868</v>
       </c>
@@ -2386,7 +2413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F48" s="3">
         <v>44869</v>
       </c>
@@ -2395,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F49" s="3">
         <v>44870</v>
       </c>
@@ -2404,21 +2431,21 @@
       </c>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F50" s="3">
         <v>44871</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F51" s="3">
         <v>44872</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F52" s="3">
         <v>44873</v>
       </c>
@@ -2435,14 +2462,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F53" s="3">
         <v>44874</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F54" s="3">
         <v>44875</v>
       </c>
@@ -2459,77 +2486,77 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="55" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F55" s="3">
         <v>44876</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F56" s="3">
         <v>44877</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F57" s="3">
         <v>44878</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F58" s="3">
         <v>44879</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F59" s="3">
         <v>44880</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F60" s="3">
         <v>44881</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F61" s="3">
         <v>44882</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
     </row>
-    <row r="62" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F62" s="3">
         <v>44883</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F63" s="3">
         <v>44884</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F64" s="3">
         <v>44885</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F65" s="3">
         <v>44886</v>
       </c>
@@ -2538,7 +2565,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="66" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F66" s="3">
         <v>44887</v>
       </c>
@@ -2555,7 +2582,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="67" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F67" s="3">
         <v>44888</v>
       </c>
@@ -2565,7 +2592,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="68" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F68" s="3">
         <v>44889</v>
       </c>
@@ -2582,21 +2609,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="69" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F69" s="3">
         <v>44890</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F70" s="3">
         <v>44891</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F71" s="3">
         <v>44892</v>
       </c>
@@ -2605,14 +2632,14 @@
       </c>
       <c r="H71" s="4"/>
     </row>
-    <row r="72" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F72" s="3">
         <v>44893</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F73" s="3">
         <v>44894</v>
       </c>
@@ -2629,14 +2656,14 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="74" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F74" s="3">
         <v>44895</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
     </row>
-    <row r="75" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F75" s="3">
         <v>44896</v>
       </c>
@@ -2651,21 +2678,21 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="76" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F76" s="3">
         <v>44897</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F77" s="3">
         <v>44898</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
     </row>
-    <row r="78" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F78" s="3">
         <v>44899</v>
       </c>
@@ -2674,7 +2701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F79" s="3">
         <v>44900</v>
       </c>
@@ -2684,7 +2711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F80" s="3">
         <v>44901</v>
       </c>
@@ -2694,7 +2721,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="81" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F81" s="3">
         <v>44902</v>
       </c>
@@ -2704,28 +2731,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F82" s="3">
         <v>44903</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F83" s="3">
         <v>44904</v>
       </c>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F84" s="3">
         <v>44905</v>
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F85" s="3">
         <v>44906</v>
       </c>
@@ -2737,7 +2764,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="86" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F86" s="3">
         <v>44907</v>
       </c>
@@ -2752,7 +2779,7 @@
         <v>4.6500000000000004</v>
       </c>
     </row>
-    <row r="87" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F87" s="3">
         <v>44908</v>
       </c>
@@ -2769,14 +2796,14 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="88" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F88" s="3">
         <v>44909</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F89" s="3">
         <v>44910</v>
       </c>
@@ -2790,7 +2817,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="90" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F90" s="3">
         <v>44911</v>
       </c>
@@ -2802,28 +2829,28 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="91" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F91" s="3">
         <v>44912</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F92" s="3">
         <v>44913</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F93" s="3">
         <v>44914</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F94" s="3">
         <v>44915</v>
       </c>
@@ -2840,7 +2867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F95" s="3">
         <v>44916</v>
       </c>
@@ -2855,7 +2882,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="96" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F96" s="3">
         <v>44917</v>
       </c>
@@ -2872,7 +2899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F97" s="3">
         <v>44918</v>
       </c>
@@ -2884,91 +2911,91 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="98" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F98" s="3">
         <v>44919</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
     </row>
-    <row r="99" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F99" s="3">
         <v>44920</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F100" s="3">
         <v>44921</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
     </row>
-    <row r="101" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F101" s="3">
         <v>44922</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F102" s="3">
         <v>44923</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
     </row>
-    <row r="103" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F103" s="3">
         <v>44924</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F104" s="3">
         <v>44925</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
     </row>
-    <row r="105" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F105" s="3">
         <v>44926</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
     </row>
-    <row r="106" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F106" s="3">
         <v>44927</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
     </row>
-    <row r="107" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F107" s="3">
         <v>44928</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
     </row>
-    <row r="108" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F108" s="3">
         <v>44929</v>
       </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F109" s="3">
         <v>44930</v>
       </c>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
     </row>
-    <row r="110" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F110" s="3">
         <v>44931</v>
       </c>
@@ -2977,21 +3004,21 @@
       </c>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F111" s="3">
         <v>44932</v>
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
     </row>
-    <row r="112" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F112" s="3">
         <v>44933</v>
       </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
     </row>
-    <row r="113" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F113" s="3">
         <v>44934</v>
       </c>
@@ -3000,7 +3027,7 @@
       </c>
       <c r="H113" s="4"/>
     </row>
-    <row r="114" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F114" s="3">
         <v>44935</v>
       </c>
@@ -3015,7 +3042,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="115" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F115" s="3">
         <v>44936</v>
       </c>
@@ -3032,7 +3059,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="116" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F116" s="3">
         <v>44937</v>
       </c>
@@ -3045,7 +3072,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="117" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F117" s="3">
         <v>44938</v>
       </c>
@@ -3062,21 +3089,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="118" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F118" s="3">
         <v>44939</v>
       </c>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
     </row>
-    <row r="119" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F119" s="3">
         <v>44940</v>
       </c>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
     </row>
-    <row r="120" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F120" s="3">
         <v>44941</v>
       </c>
@@ -3085,7 +3112,7 @@
       </c>
       <c r="H120" s="4"/>
     </row>
-    <row r="121" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F121" s="3">
         <v>44942</v>
       </c>
@@ -3102,7 +3129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F122" s="3">
         <v>44943</v>
       </c>
@@ -3119,7 +3146,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="123" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F123" s="3">
         <v>44944</v>
       </c>
@@ -3128,7 +3155,7 @@
       </c>
       <c r="H123" s="4"/>
     </row>
-    <row r="124" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F124" s="3">
         <v>44945</v>
       </c>
@@ -3145,7 +3172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F125" s="3">
         <v>44946</v>
       </c>
@@ -3162,7 +3189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F126" s="3">
         <v>44947</v>
       </c>
@@ -3172,107 +3199,129 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F127" s="3">
         <v>44948</v>
       </c>
-      <c r="G127" s="4"/>
+      <c r="G127" s="4">
+        <v>2.25</v>
+      </c>
       <c r="H127" s="4"/>
     </row>
-    <row r="128" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F128" s="3">
         <v>44949</v>
       </c>
-      <c r="G128" s="4"/>
-      <c r="H128" s="4"/>
-    </row>
-    <row r="129" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="G128" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="H128" s="4">
+        <v>4</v>
+      </c>
+      <c r="I128">
+        <v>5.5</v>
+      </c>
+      <c r="J128">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="129" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F129" s="3">
         <v>44950</v>
       </c>
-      <c r="G129" s="4"/>
-      <c r="H129" s="4"/>
-    </row>
-    <row r="130" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="G129" s="4">
+        <v>2</v>
+      </c>
+      <c r="H129" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="I129">
+        <v>3.5</v>
+      </c>
+      <c r="J129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F130" s="3">
         <v>44951</v>
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="4"/>
     </row>
-    <row r="131" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F131" s="3"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
     </row>
-    <row r="132" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F132" s="3"/>
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
     </row>
-    <row r="133" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F133" s="3"/>
       <c r="G133" s="4"/>
       <c r="H133" s="4"/>
     </row>
-    <row r="134" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F134" s="3"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
     </row>
-    <row r="135" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F135" s="3"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
     </row>
-    <row r="136" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F136" s="3"/>
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
     </row>
-    <row r="137" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F137" s="3"/>
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
     </row>
-    <row r="138" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F138" s="3"/>
     </row>
-    <row r="139" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E139" s="7" t="s">
+    <row r="139" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E139" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F139" s="7"/>
-      <c r="G139" s="8">
+      <c r="F139" s="8"/>
+      <c r="G139" s="6">
         <f>SUM(G5,G5:G137)</f>
-        <v>73.199999999999989</v>
-      </c>
-      <c r="H139" s="8">
+        <v>82.949999999999989</v>
+      </c>
+      <c r="H139" s="6">
         <f>SUM(H5,H6:H138)</f>
-        <v>47.849999999999994</v>
-      </c>
-      <c r="I139" s="8">
+        <v>55.349999999999994</v>
+      </c>
+      <c r="I139" s="6">
         <f>SUM(I5,I6:I138)</f>
-        <v>63.75</v>
-      </c>
-      <c r="J139" s="8">
+        <v>72.75</v>
+      </c>
+      <c r="J139" s="6">
         <f>SUM(J5,J6:J138)</f>
-        <v>93.85</v>
-      </c>
-      <c r="L139" s="8" t="s">
+        <v>101.35</v>
+      </c>
+      <c r="L139" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="L140" s="8"/>
-    </row>
-    <row r="141" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="L140" s="6"/>
+    </row>
+    <row r="141" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E141" s="9" t="s">
         <v>4</v>
       </c>
@@ -3289,50 +3338,45 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="8"/>
-    </row>
-    <row r="142" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E142" s="8" t="s">
+      <c r="L141" s="6"/>
+    </row>
+    <row r="142" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E142" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8">
+      <c r="F142" s="6"/>
+      <c r="G142" s="6">
         <f>PRODUCT(G139,G141)</f>
-        <v>1143.7499999999998</v>
-      </c>
-      <c r="H142" s="8">
+        <v>1296.0937499999998</v>
+      </c>
+      <c r="H142" s="6">
         <f>PRODUCT(H139,H141)</f>
-        <v>747.65624999999989</v>
-      </c>
-      <c r="I142" s="8">
+        <v>864.84374999999989</v>
+      </c>
+      <c r="I142" s="6">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
-        <v>996.09375</v>
-      </c>
-      <c r="J142" s="8">
+        <v>1136.71875</v>
+      </c>
+      <c r="J142" s="6">
         <f t="shared" si="0"/>
-        <v>1466.40625</v>
-      </c>
-      <c r="L142" s="8">
+        <v>1583.59375</v>
+      </c>
+      <c r="L142" s="6">
         <f>SUM(G142:J143)</f>
-        <v>4353.90625</v>
-      </c>
-    </row>
-    <row r="143" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8"/>
-      <c r="L143" s="8"/>
+        <v>4881.25</v>
+      </c>
+    </row>
+    <row r="143" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="L143" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -3342,6 +3386,11 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>